<commit_message>
Add disease_profile fields in lung template
</commit_message>
<xml_diff>
--- a/template/hca_lung_template.xlsx
+++ b/template/hca_lung_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2EBBAF-3640-9743-B844-96F2339F4280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBABA55-D23A-D043-BBA0-BEEB420BB3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="17600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4880" yWindow="500" windowWidth="41440" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="1725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3274" uniqueCount="1749">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -5237,6 +5237,78 @@
   </si>
   <si>
     <t>KCO PERCENT OF PREDICTED</t>
+  </si>
+  <si>
+    <t>donor_organism.disease_profile.copd_gold_stage</t>
+  </si>
+  <si>
+    <t>Indicate the Modified British Medical Research Council (mMRC) dyspnea scale grade</t>
+  </si>
+  <si>
+    <t>Should be one of 0, 1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>donor_organism.disease_profile.copd_cat_score</t>
+  </si>
+  <si>
+    <t>Should be between 0 and 40</t>
+  </si>
+  <si>
+    <t>Indicate the COPD Assessment Test (CAT) score.</t>
+  </si>
+  <si>
+    <t>Indicate the current GOLD stage (Global Initiative for Chronic Obstructive Lung Disease).</t>
+  </si>
+  <si>
+    <t>Should be one of 1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>COPD - CAT SCORE</t>
+  </si>
+  <si>
+    <t>COPD - MMRC GRADE</t>
+  </si>
+  <si>
+    <t>COPD - GOLD STAGE</t>
+  </si>
+  <si>
+    <t>COPD - GOLD ABE ASSESSMENT</t>
+  </si>
+  <si>
+    <t>Indicate the Global Initiative for Chronic Obstructive Lung Disease (GOLD) A, B, C, D assessment group if available.</t>
+  </si>
+  <si>
+    <t>Should be one of A, B, E</t>
+  </si>
+  <si>
+    <t>donor_organism.disease_profile.copd_phenotype</t>
+  </si>
+  <si>
+    <t>donor_organism.disease_profile.copd_gold_abe_assessment</t>
+  </si>
+  <si>
+    <t>Indicate the COPD disease phenotype(s) of donor. Please indicate all applicable phenotypes of donor.</t>
+  </si>
+  <si>
+    <t>Should be one or more of: COPD not otherwise specified, COPD with emphysema, COPD with bronchitis, COPD with history of asthma, COPD with &gt;300 eos in blood, COPD with allergy, COPD with Chronic Mucus Hypersecretion, COPD with frequent exacerbations</t>
+  </si>
+  <si>
+    <t>Indicate the percentage of the lung that is affected by emphysema as judged based on non-invasive imaging, such as from a CT scan.</t>
+  </si>
+  <si>
+    <t>COPD PHENOTYPE</t>
+  </si>
+  <si>
+    <t>COPD - PERCENTAGE OF EMPHYSEMA</t>
+  </si>
+  <si>
+    <t>donor_organism.disease_profile.copd_emphysema_percentage</t>
+  </si>
+  <si>
+    <t>For example: 93; 85; 77</t>
+  </si>
+  <si>
+    <t>donor_organism.disease_profile.copd_mmrc_grade</t>
   </si>
 </sst>
 </file>
@@ -5645,7 +5717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13436,9 +13508,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:DN5"/>
+  <dimension ref="A1:DE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13498,16 +13570,17 @@
     <col min="84" max="84" width="13.83203125" customWidth="1"/>
     <col min="85" max="85" width="15" customWidth="1"/>
     <col min="86" max="86" width="11.83203125" customWidth="1"/>
-    <col min="87" max="87" width="16.6640625" customWidth="1"/>
-    <col min="88" max="96" width="25.6640625" customWidth="1"/>
-    <col min="97" max="98" width="8.83203125" customWidth="1"/>
-    <col min="99" max="99" width="25.6640625" customWidth="1"/>
-    <col min="100" max="101" width="8.83203125" customWidth="1"/>
-    <col min="102" max="102" width="25.6640625" customWidth="1"/>
-    <col min="103" max="103" width="37.6640625" customWidth="1"/>
+    <col min="87" max="92" width="16.6640625" customWidth="1"/>
+    <col min="93" max="93" width="19.5" customWidth="1"/>
+    <col min="94" max="102" width="25.6640625" customWidth="1"/>
+    <col min="103" max="104" width="8.83203125" customWidth="1"/>
+    <col min="105" max="105" width="25.6640625" customWidth="1"/>
+    <col min="106" max="107" width="8.83203125" customWidth="1"/>
+    <col min="108" max="108" width="25.6640625" customWidth="1"/>
+    <col min="109" max="109" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
@@ -13769,56 +13842,74 @@
       <c r="CI1" s="3" t="s">
         <v>1724</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CJ1" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="CK1" s="3" t="s">
+        <v>1734</v>
+      </c>
+      <c r="CL1" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="CM1" s="3" t="s">
+        <v>1736</v>
+      </c>
+      <c r="CN1" s="3" t="s">
+        <v>1744</v>
+      </c>
+      <c r="CO1" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="CP1" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:103" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:109" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -14081,55 +14172,73 @@
         <v>1650</v>
       </c>
       <c r="CJ2" s="2" t="s">
+        <v>1731</v>
+      </c>
+      <c r="CK2" s="2" t="s">
+        <v>1726</v>
+      </c>
+      <c r="CL2" s="2" t="s">
+        <v>1730</v>
+      </c>
+      <c r="CM2" s="2" t="s">
+        <v>1737</v>
+      </c>
+      <c r="CN2" s="2" t="s">
+        <v>1741</v>
+      </c>
+      <c r="CO2" s="2" t="s">
+        <v>1743</v>
+      </c>
+      <c r="CP2" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="CK2" s="2" t="s">
+      <c r="CQ2" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="CL2" s="2" t="s">
+      <c r="CR2" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="CM2" s="2" t="s">
+      <c r="CS2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="CN2" s="2" t="s">
+      <c r="CT2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CU2" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="CP2" s="2" t="s">
+      <c r="CV2" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="CQ2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="CR2" s="2" t="s">
+      <c r="CX2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="CS2" s="2" t="s">
+      <c r="CY2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="CT2" s="2" t="s">
+      <c r="CZ2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CU2" s="2" t="s">
+      <c r="DA2" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="CV2" s="2" t="s">
+      <c r="DB2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="CW2" s="2" t="s">
+      <c r="DC2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CX2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="CY2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:103" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:109" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -14385,50 +14494,68 @@
       <c r="CI3" s="2" t="s">
         <v>1676</v>
       </c>
-      <c r="CJ3" s="2"/>
-      <c r="CK3" s="2"/>
-      <c r="CL3" s="2"/>
+      <c r="CJ3" s="2" t="s">
+        <v>1732</v>
+      </c>
+      <c r="CK3" s="2" t="s">
+        <v>1727</v>
+      </c>
+      <c r="CL3" s="2" t="s">
+        <v>1729</v>
+      </c>
       <c r="CM3" s="2" t="s">
+        <v>1738</v>
+      </c>
+      <c r="CN3" s="2" t="s">
+        <v>1742</v>
+      </c>
+      <c r="CO3" s="2" t="s">
+        <v>1747</v>
+      </c>
+      <c r="CP3" s="2"/>
+      <c r="CQ3" s="2"/>
+      <c r="CR3" s="2"/>
+      <c r="CS3" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="CN3" s="2" t="s">
+      <c r="CT3" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="CO3" s="2" t="s">
+      <c r="CU3" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="CP3" s="2" t="s">
+      <c r="CV3" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="CQ3" s="2" t="s">
+      <c r="CW3" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="CR3" s="2" t="s">
+      <c r="CX3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="CS3" s="2" t="s">
+      <c r="CY3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="CT3" s="2" t="s">
+      <c r="CZ3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="CU3" s="2" t="s">
+      <c r="DA3" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="CV3" s="2" t="s">
+      <c r="DB3" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="CW3" s="2" t="s">
+      <c r="DC3" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="CX3" s="2" t="s">
+      <c r="DD3" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="CY3" s="2" t="s">
+      <c r="DE3" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:109" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -14691,55 +14818,73 @@
         <v>1702</v>
       </c>
       <c r="CJ4" t="s">
+        <v>1725</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>1748</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>1728</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>1740</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>1739</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>1746</v>
+      </c>
+      <c r="CP4" t="s">
         <v>316</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CQ4" t="s">
         <v>319</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CR4" t="s">
         <v>322</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CS4" t="s">
         <v>326</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CT4" t="s">
         <v>330</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CU4" t="s">
         <v>334</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CV4" t="s">
         <v>337</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CW4" t="s">
         <v>341</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CX4" t="s">
         <v>343</v>
       </c>
-      <c r="CS4" t="s">
+      <c r="CY4" t="s">
         <v>345</v>
       </c>
-      <c r="CT4" t="s">
+      <c r="CZ4" t="s">
         <v>347</v>
       </c>
-      <c r="CU4" t="s">
+      <c r="DA4" t="s">
         <v>351</v>
       </c>
-      <c r="CV4" t="s">
+      <c r="DB4" t="s">
         <v>354</v>
       </c>
-      <c r="CW4" t="s">
+      <c r="DC4" t="s">
         <v>356</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="DD4" t="s">
         <v>360</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="DE4" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="5" spans="1:103" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -14845,6 +14990,12 @@
       <c r="CW5" s="1"/>
       <c r="CX5" s="1"/>
       <c r="CY5" s="1"/>
+      <c r="CZ5" s="1"/>
+      <c r="DA5" s="1"/>
+      <c r="DB5" s="1"/>
+      <c r="DC5" s="1"/>
+      <c r="DD5" s="1"/>
+      <c r="DE5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added missing permebilisation_time fields in imaging_preparation_protocol
</commit_message>
<xml_diff>
--- a/template/hca_lung_template.xlsx
+++ b/template/hca_lung_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBABA55-D23A-D043-BBA0-BEEB420BB3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F76ADF3-CDA6-7447-A5CD-119BA0AB8553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="500" windowWidth="41440" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3274" uniqueCount="1749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3280" uniqueCount="1754">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -5309,13 +5309,28 @@
   </si>
   <si>
     <t>donor_organism.disease_profile.copd_mmrc_grade</t>
+  </si>
+  <si>
+    <t>The permeabilisation time in time units that the tissue was exposed to.</t>
+  </si>
+  <si>
+    <t>The unit in which permeabilisation time is expressed.</t>
+  </si>
+  <si>
+    <t>For example: 3; 12; 42</t>
+  </si>
+  <si>
+    <t>imaging_preparation_protocol.permeabilisation_time</t>
+  </si>
+  <si>
+    <t>imaging_preparation_protocol.permeabilisation_time_unit.text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5359,6 +5374,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5383,10 +5405,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5411,9 +5434,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{3FF3C3F0-5B10-3546-8AF6-D8C852BC6338}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -10792,7 +10823,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10812,9 +10843,11 @@
     <col min="21" max="21" width="37.6640625" customWidth="1"/>
     <col min="22" max="23" width="0" hidden="1" customWidth="1"/>
     <col min="24" max="25" width="25.6640625" customWidth="1"/>
+    <col min="26" max="26" width="24.5" customWidth="1"/>
+    <col min="27" max="27" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>686</v>
       </c>
@@ -10890,8 +10923,16 @@
       <c r="Y1" s="1" t="s">
         <v>1075</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z1" s="10" t="str">
+        <f>UPPER("Permeabilisation time")</f>
+        <v>PERMEABILISATION TIME</v>
+      </c>
+      <c r="AA1" s="10" t="str">
+        <f>UPPER("Permeabilisation time unit")</f>
+        <v>PERMEABILISATION TIME UNIT</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>481</v>
       </c>
@@ -10967,8 +11008,14 @@
       <c r="Y2" s="2" t="s">
         <v>1076</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z2" s="11" t="s">
+        <v>1749</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>482</v>
       </c>
@@ -11040,8 +11087,14 @@
       <c r="Y3" s="2" t="s">
         <v>1077</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z3" s="11" t="s">
+        <v>1751</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>687</v>
       </c>
@@ -11117,8 +11170,14 @@
       <c r="Y4" t="s">
         <v>1078</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z4" s="12" t="s">
+        <v>1752</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -11146,6 +11205,8 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added atlas names & fixed function in permebilisation
</commit_message>
<xml_diff>
--- a/template/hca_lung_template.xlsx
+++ b/template/hca_lung_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F76ADF3-CDA6-7447-A5CD-119BA0AB8553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9705D13-41DE-904B-9C85-9923BA18A2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14920" yWindow="5860" windowWidth="21360" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3280" uniqueCount="1754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="1756">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -4702,9 +4702,6 @@
     <t xml:space="preserve">A field describing if the project is part of a HCA Tissue Atlas (e.g. Brain Alzheimer Atlas). </t>
   </si>
   <si>
-    <t>For example: Blood Atlas</t>
-  </si>
-  <si>
     <t>OFFICIAL HCA TISSUE ATLAS VERSION</t>
   </si>
   <si>
@@ -5324,6 +5321,15 @@
   </si>
   <si>
     <t>imaging_preparation_protocol.permeabilisation_time_unit.text</t>
+  </si>
+  <si>
+    <t>Should be of: Adipose, Brain, Breast, Development, Eye, GDN, Gut, Heart, Immune, Kidney, Liver, Lung, MSK, ORCF, Organoid-Endoderm, Organoid-Neural, Pancreas Retina, Reproduction, Skin</t>
+  </si>
+  <si>
+    <t>PERMEABILISATION TIME</t>
+  </si>
+  <si>
+    <t>PERMEABILISATION TIME UNIT</t>
   </si>
 </sst>
 </file>
@@ -5409,7 +5415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5441,6 +5447,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5801,10 +5810,10 @@
         <v>568</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>1541</v>
@@ -5813,10 +5822,10 @@
         <v>1544</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -5857,10 +5866,10 @@
         <v>1462</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>1542</v>
@@ -5869,10 +5878,10 @@
         <v>1545</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -5913,22 +5922,22 @@
         <v>1463</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>1543</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>1546</v>
+      <c r="P3" s="13" t="s">
+        <v>1753</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5969,22 +5978,22 @@
         <v>1461</v>
       </c>
       <c r="M4" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="N4" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="O4" t="s">
+        <v>1552</v>
+      </c>
+      <c r="P4" t="s">
         <v>1553</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>1554</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>1555</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1556</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6948,19 +6957,19 @@
         <v>787</v>
       </c>
       <c r="BE4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="BF4" t="s">
         <v>1577</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BG4" t="s">
         <v>1578</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>1579</v>
       </c>
-      <c r="BH4" t="s">
-        <v>1580</v>
-      </c>
       <c r="BI4" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="BJ4" t="s">
         <v>366</v>
@@ -7500,7 +7509,7 @@
         <v>833</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>837</v>
@@ -7598,7 +7607,7 @@
         <v>834</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>838</v>
@@ -7696,7 +7705,7 @@
         <v>835</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>839</v>
@@ -7786,7 +7795,7 @@
         <v>836</v>
       </c>
       <c r="L4" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="M4" t="s">
         <v>840</v>
@@ -10923,13 +10932,11 @@
       <c r="Y1" s="1" t="s">
         <v>1075</v>
       </c>
-      <c r="Z1" s="10" t="str">
-        <f>UPPER("Permeabilisation time")</f>
-        <v>PERMEABILISATION TIME</v>
-      </c>
-      <c r="AA1" s="10" t="str">
-        <f>UPPER("Permeabilisation time unit")</f>
-        <v>PERMEABILISATION TIME UNIT</v>
+      <c r="Z1" s="10" t="s">
+        <v>1754</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>1755</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -11009,10 +11016,10 @@
         <v>1076</v>
       </c>
       <c r="Z2" s="11" t="s">
+        <v>1748</v>
+      </c>
+      <c r="AA2" s="11" t="s">
         <v>1749</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>1750</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="80" customHeight="1" x14ac:dyDescent="0.2">
@@ -11088,7 +11095,7 @@
         <v>1077</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="AA3" s="11" t="s">
         <v>195</v>
@@ -11171,10 +11178,10 @@
         <v>1078</v>
       </c>
       <c r="Z4" s="12" t="s">
+        <v>1751</v>
+      </c>
+      <c r="AA4" s="12" t="s">
         <v>1752</v>
-      </c>
-      <c r="AA4" s="12" t="s">
-        <v>1753</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -12623,16 +12630,16 @@
         <v>1421</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>1422</v>
@@ -12674,16 +12681,16 @@
         <v>78</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>1523</v>
@@ -12718,19 +12725,19 @@
         <v>353</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>1524</v>
@@ -12772,16 +12779,16 @@
         <v>1436</v>
       </c>
       <c r="I4" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="J4" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="K4" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="L4" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="M4" t="s">
         <v>1437</v>
@@ -13826,100 +13833,100 @@
         <v>311</v>
       </c>
       <c r="BJ1" s="3" t="s">
+        <v>1702</v>
+      </c>
+      <c r="BK1" s="3" t="s">
         <v>1703</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>1704</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>1705</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>1706</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>1707</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>1708</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>1709</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>1710</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>1711</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>1712</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>1713</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>1714</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>1715</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>1716</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>1717</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>1718</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>1719</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
+        <v>1620</v>
+      </c>
+      <c r="CC1" s="3" t="s">
         <v>1720</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>1621</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>1721</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>1622</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>1722</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>1623</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>1723</v>
       </c>
-      <c r="CH1" s="3" t="s">
-        <v>1624</v>
-      </c>
-      <c r="CI1" s="3" t="s">
-        <v>1724</v>
-      </c>
       <c r="CJ1" s="3" t="s">
+        <v>1734</v>
+      </c>
+      <c r="CK1" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="CL1" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="CM1" s="3" t="s">
         <v>1735</v>
       </c>
-      <c r="CK1" s="3" t="s">
-        <v>1734</v>
-      </c>
-      <c r="CL1" s="3" t="s">
-        <v>1733</v>
-      </c>
-      <c r="CM1" s="3" t="s">
-        <v>1736</v>
-      </c>
       <c r="CN1" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="CO1" s="3" t="s">
         <v>1744</v>
-      </c>
-      <c r="CO1" s="3" t="s">
-        <v>1745</v>
       </c>
       <c r="CP1" s="1" t="s">
         <v>314</v>
@@ -14155,100 +14162,100 @@
         <v>312</v>
       </c>
       <c r="BJ2" s="2" t="s">
+        <v>1624</v>
+      </c>
+      <c r="BK2" s="2" t="s">
         <v>1625</v>
       </c>
-      <c r="BK2" s="2" t="s">
+      <c r="BL2" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="BL2" s="2" t="s">
+      <c r="BM2" s="2" t="s">
         <v>1627</v>
       </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BN2" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
         <v>1629</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BP2" s="2" t="s">
         <v>1630</v>
       </c>
-      <c r="BP2" s="2" t="s">
+      <c r="BQ2" s="2" t="s">
         <v>1631</v>
       </c>
-      <c r="BQ2" s="2" t="s">
+      <c r="BR2" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="BR2" s="2" t="s">
+      <c r="BS2" s="2" t="s">
         <v>1633</v>
       </c>
-      <c r="BS2" s="2" t="s">
+      <c r="BT2" s="2" t="s">
         <v>1634</v>
       </c>
-      <c r="BT2" s="2" t="s">
+      <c r="BU2" s="2" t="s">
         <v>1635</v>
       </c>
-      <c r="BU2" s="2" t="s">
+      <c r="BV2" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BW2" s="2" t="s">
         <v>1637</v>
       </c>
-      <c r="BW2" s="2" t="s">
+      <c r="BX2" s="2" t="s">
         <v>1638</v>
       </c>
-      <c r="BX2" s="2" t="s">
+      <c r="BY2" s="2" t="s">
         <v>1639</v>
       </c>
-      <c r="BY2" s="2" t="s">
+      <c r="BZ2" s="2" t="s">
         <v>1640</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CA2" s="2" t="s">
         <v>1641</v>
       </c>
-      <c r="CA2" s="2" t="s">
+      <c r="CB2" s="2" t="s">
         <v>1642</v>
       </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CC2" s="2" t="s">
         <v>1643</v>
       </c>
-      <c r="CC2" s="2" t="s">
+      <c r="CD2" s="2" t="s">
         <v>1644</v>
       </c>
-      <c r="CD2" s="2" t="s">
+      <c r="CE2" s="2" t="s">
         <v>1645</v>
       </c>
-      <c r="CE2" s="2" t="s">
+      <c r="CF2" s="2" t="s">
         <v>1646</v>
       </c>
-      <c r="CF2" s="2" t="s">
+      <c r="CG2" s="2" t="s">
         <v>1647</v>
       </c>
-      <c r="CG2" s="2" t="s">
+      <c r="CH2" s="2" t="s">
         <v>1648</v>
       </c>
-      <c r="CH2" s="2" t="s">
+      <c r="CI2" s="2" t="s">
         <v>1649</v>
       </c>
-      <c r="CI2" s="2" t="s">
-        <v>1650</v>
-      </c>
       <c r="CJ2" s="2" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="CK2" s="2" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="CL2" s="2" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="CM2" s="2" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="CN2" s="2" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="CO2" s="2" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="CP2" s="2" t="s">
         <v>315</v>
@@ -14478,100 +14485,100 @@
         <v>313</v>
       </c>
       <c r="BJ3" s="2" t="s">
+        <v>1650</v>
+      </c>
+      <c r="BK3" s="2" t="s">
         <v>1651</v>
       </c>
-      <c r="BK3" s="2" t="s">
+      <c r="BL3" s="2" t="s">
         <v>1652</v>
       </c>
-      <c r="BL3" s="2" t="s">
+      <c r="BM3" s="2" t="s">
         <v>1653</v>
       </c>
-      <c r="BM3" s="2" t="s">
+      <c r="BN3" s="2" t="s">
         <v>1654</v>
       </c>
-      <c r="BN3" s="2" t="s">
+      <c r="BO3" s="2" t="s">
         <v>1655</v>
       </c>
-      <c r="BO3" s="2" t="s">
+      <c r="BP3" s="2" t="s">
         <v>1656</v>
       </c>
-      <c r="BP3" s="2" t="s">
+      <c r="BQ3" s="2" t="s">
         <v>1657</v>
       </c>
-      <c r="BQ3" s="2" t="s">
+      <c r="BR3" s="2" t="s">
         <v>1658</v>
       </c>
-      <c r="BR3" s="2" t="s">
+      <c r="BS3" s="2" t="s">
         <v>1659</v>
       </c>
-      <c r="BS3" s="2" t="s">
+      <c r="BT3" s="2" t="s">
         <v>1660</v>
       </c>
-      <c r="BT3" s="2" t="s">
+      <c r="BU3" s="2" t="s">
         <v>1661</v>
       </c>
-      <c r="BU3" s="2" t="s">
+      <c r="BV3" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="BV3" s="2" t="s">
+      <c r="BW3" s="2" t="s">
         <v>1663</v>
       </c>
-      <c r="BW3" s="2" t="s">
+      <c r="BX3" s="2" t="s">
         <v>1664</v>
       </c>
-      <c r="BX3" s="2" t="s">
+      <c r="BY3" s="2" t="s">
         <v>1665</v>
       </c>
-      <c r="BY3" s="2" t="s">
+      <c r="BZ3" s="2" t="s">
         <v>1666</v>
       </c>
-      <c r="BZ3" s="2" t="s">
+      <c r="CA3" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="CA3" s="2" t="s">
+      <c r="CB3" s="2" t="s">
         <v>1668</v>
       </c>
-      <c r="CB3" s="2" t="s">
+      <c r="CC3" s="2" t="s">
         <v>1669</v>
       </c>
-      <c r="CC3" s="2" t="s">
+      <c r="CD3" s="2" t="s">
         <v>1670</v>
       </c>
-      <c r="CD3" s="2" t="s">
+      <c r="CE3" s="2" t="s">
         <v>1671</v>
       </c>
-      <c r="CE3" s="2" t="s">
+      <c r="CF3" s="2" t="s">
         <v>1672</v>
       </c>
-      <c r="CF3" s="2" t="s">
+      <c r="CG3" s="2" t="s">
         <v>1673</v>
       </c>
-      <c r="CG3" s="2" t="s">
+      <c r="CH3" s="2" t="s">
         <v>1674</v>
       </c>
-      <c r="CH3" s="2" t="s">
+      <c r="CI3" s="2" t="s">
         <v>1675</v>
       </c>
-      <c r="CI3" s="2" t="s">
-        <v>1676</v>
-      </c>
       <c r="CJ3" s="2" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="CK3" s="2" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="CL3" s="2" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="CM3" s="2" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="CN3" s="2" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="CO3" s="2" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="CP3" s="2"/>
       <c r="CQ3" s="2"/>
@@ -14786,115 +14793,115 @@
         <v>304</v>
       </c>
       <c r="BE4" t="s">
+        <v>1556</v>
+      </c>
+      <c r="BF4" t="s">
         <v>1557</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BG4" t="s">
         <v>1558</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
         <v>1559</v>
       </c>
-      <c r="BH4" t="s">
-        <v>1560</v>
-      </c>
       <c r="BI4" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="BJ4" t="s">
+        <v>1676</v>
+      </c>
+      <c r="BK4" t="s">
         <v>1677</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>1678</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BM4" t="s">
         <v>1679</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BN4" t="s">
         <v>1680</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="BO4" t="s">
         <v>1681</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
         <v>1682</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BQ4" t="s">
         <v>1683</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BR4" t="s">
         <v>1684</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="BS4" t="s">
         <v>1685</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="BT4" t="s">
         <v>1686</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BU4" t="s">
         <v>1687</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="BV4" t="s">
         <v>1688</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="BW4" t="s">
         <v>1689</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="BX4" t="s">
         <v>1690</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="BY4" t="s">
         <v>1691</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" t="s">
         <v>1692</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CA4" t="s">
         <v>1693</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CB4" t="s">
         <v>1694</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CC4" t="s">
         <v>1695</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
         <v>1696</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CE4" t="s">
         <v>1697</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CF4" t="s">
         <v>1698</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CG4" t="s">
         <v>1699</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CH4" t="s">
         <v>1700</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CI4" t="s">
         <v>1701</v>
       </c>
-      <c r="CI4" t="s">
-        <v>1702</v>
-      </c>
       <c r="CJ4" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="CK4" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="CL4" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="CM4" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="CN4" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="CO4" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="CP4" t="s">
         <v>316</v>
@@ -15164,7 +15171,7 @@
         <v>396</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>211</v>
@@ -15373,7 +15380,7 @@
         <v>78</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>398</v>
@@ -15771,13 +15778,13 @@
         <v>393</v>
       </c>
       <c r="Q4" t="s">
+        <v>1610</v>
+      </c>
+      <c r="R4" t="s">
         <v>1611</v>
       </c>
-      <c r="R4" t="s">
-        <v>1612</v>
-      </c>
       <c r="S4" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="T4" t="s">
         <v>399</v>
@@ -15840,19 +15847,19 @@
         <v>451</v>
       </c>
       <c r="AN4" t="s">
+        <v>1560</v>
+      </c>
+      <c r="AO4" t="s">
         <v>1561</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>1562</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>1563</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>1564</v>
-      </c>
       <c r="AR4" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="AS4" t="s">
         <v>454</v>
@@ -16682,19 +16689,19 @@
         <v>583</v>
       </c>
       <c r="AJ4" t="s">
+        <v>1564</v>
+      </c>
+      <c r="AK4" t="s">
         <v>1565</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>1566</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>1567</v>
       </c>
-      <c r="AM4" t="s">
-        <v>1568</v>
-      </c>
       <c r="AN4" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="AO4" t="s">
         <v>366</v>
@@ -17378,19 +17385,19 @@
         <v>600</v>
       </c>
       <c r="J4" t="s">
+        <v>1568</v>
+      </c>
+      <c r="K4" t="s">
         <v>1569</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>1570</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>1571</v>
       </c>
-      <c r="M4" t="s">
-        <v>1572</v>
-      </c>
       <c r="N4" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="O4" t="s">
         <v>602</v>
@@ -17584,7 +17591,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17977,19 +17986,19 @@
         <v>685</v>
       </c>
       <c r="O4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="P4" t="s">
         <v>1573</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>1574</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>1575</v>
       </c>
-      <c r="R4" t="s">
-        <v>1576</v>
-      </c>
       <c r="S4" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="T4" t="s">
         <v>366</v>

</xml_diff>

<commit_message>
Add gender identity field
</commit_message>
<xml_diff>
--- a/template/hca_lung_template.xlsx
+++ b/template/hca_lung_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37B8E54-EB9C-3D48-B021-0CF753A1DB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA0BA11-1EFD-A545-8315-FBAE8436EB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4960" yWindow="760" windowWidth="21360" windowHeight="17600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3310" uniqueCount="1779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="1788">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -5399,6 +5399,33 @@
   </si>
   <si>
     <t>donor_organism.medical_history.medication.ontology_label</t>
+  </si>
+  <si>
+    <t>GENDER IDENTITY</t>
+  </si>
+  <si>
+    <t>GENDER IDENTITY ONTOLOGY</t>
+  </si>
+  <si>
+    <t>GENDER IDENTITY ONTOLOGY ID</t>
+  </si>
+  <si>
+    <t>The donor's personal sense of their own gender at the time of the experiment.</t>
+  </si>
+  <si>
+    <t>For example: Female Gender; Agender; Non-Binary Gender</t>
+  </si>
+  <si>
+    <t>For example: NCIT:C46110; NCIT:C205469; NCIT:C160941</t>
+  </si>
+  <si>
+    <t>donor_organism.gender_identity.text</t>
+  </si>
+  <si>
+    <t>donor_organism.gender_identity.ontology</t>
+  </si>
+  <si>
+    <t>donor_organism.gender_identity.ontology_label</t>
   </si>
 </sst>
 </file>
@@ -13663,10 +13690,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:DL5"/>
+  <dimension ref="A1:DO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ2" sqref="AQ2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5:W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13680,68 +13707,69 @@
     <col min="15" max="16" width="0" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="25.6640625" customWidth="1"/>
     <col min="18" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="25.6640625" customWidth="1"/>
-    <col min="21" max="21" width="30.6640625" customWidth="1"/>
-    <col min="22" max="23" width="25.6640625" customWidth="1"/>
-    <col min="24" max="25" width="0" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="28.6640625" customWidth="1"/>
+    <col min="20" max="21" width="25.6640625" customWidth="1"/>
+    <col min="22" max="23" width="15.83203125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="30.6640625" customWidth="1"/>
+    <col min="25" max="26" width="25.6640625" customWidth="1"/>
     <col min="27" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.6640625" customWidth="1"/>
-    <col min="30" max="31" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="21.6640625" customWidth="1"/>
+    <col min="29" max="29" width="28.6640625" customWidth="1"/>
+    <col min="30" max="31" width="0" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="25.6640625" customWidth="1"/>
     <col min="33" max="34" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="35" max="36" width="25.6640625" customWidth="1"/>
-    <col min="37" max="37" width="28.6640625" customWidth="1"/>
-    <col min="38" max="40" width="25.6640625" customWidth="1"/>
-    <col min="41" max="41" width="31.6640625" customWidth="1"/>
-    <col min="42" max="43" width="25.6640625" customWidth="1"/>
-    <col min="44" max="45" width="11.1640625" hidden="1" customWidth="1"/>
-    <col min="46" max="50" width="25.6640625" customWidth="1"/>
-    <col min="51" max="52" width="0" hidden="1" customWidth="1"/>
-    <col min="53" max="54" width="25.6640625" customWidth="1"/>
-    <col min="55" max="56" width="0" hidden="1" customWidth="1"/>
-    <col min="57" max="58" width="25.6640625" customWidth="1"/>
-    <col min="59" max="60" width="0" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="27.6640625" customWidth="1"/>
-    <col min="62" max="62" width="26.6640625" customWidth="1"/>
-    <col min="63" max="64" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="25.6640625" customWidth="1"/>
-    <col min="66" max="66" width="23.33203125" customWidth="1"/>
-    <col min="67" max="67" width="20.6640625" customWidth="1"/>
-    <col min="68" max="68" width="20.33203125" customWidth="1"/>
-    <col min="69" max="69" width="32" customWidth="1"/>
-    <col min="70" max="70" width="16.1640625" customWidth="1"/>
-    <col min="71" max="71" width="21.5" customWidth="1"/>
-    <col min="72" max="72" width="18.83203125" customWidth="1"/>
-    <col min="73" max="73" width="19" customWidth="1"/>
-    <col min="74" max="74" width="18.83203125" customWidth="1"/>
-    <col min="75" max="75" width="16.1640625" customWidth="1"/>
-    <col min="76" max="76" width="18.33203125" customWidth="1"/>
-    <col min="77" max="77" width="18.6640625" customWidth="1"/>
-    <col min="78" max="78" width="19.5" customWidth="1"/>
-    <col min="79" max="79" width="19.33203125" customWidth="1"/>
-    <col min="80" max="80" width="24.83203125" customWidth="1"/>
-    <col min="81" max="81" width="23.5" customWidth="1"/>
-    <col min="82" max="82" width="17" customWidth="1"/>
-    <col min="83" max="83" width="16.6640625" customWidth="1"/>
-    <col min="84" max="84" width="12.5" customWidth="1"/>
-    <col min="85" max="85" width="15.33203125" customWidth="1"/>
-    <col min="86" max="86" width="13.5" customWidth="1"/>
-    <col min="87" max="87" width="15.33203125" customWidth="1"/>
-    <col min="88" max="88" width="13.83203125" customWidth="1"/>
-    <col min="89" max="89" width="15" customWidth="1"/>
-    <col min="90" max="90" width="11.83203125" customWidth="1"/>
-    <col min="91" max="96" width="16.6640625" customWidth="1"/>
-    <col min="97" max="97" width="19.5" customWidth="1"/>
-    <col min="98" max="106" width="25.6640625" customWidth="1"/>
-    <col min="107" max="108" width="8.83203125" customWidth="1"/>
-    <col min="109" max="109" width="25.6640625" customWidth="1"/>
+    <col min="35" max="35" width="21.6640625" customWidth="1"/>
+    <col min="36" max="37" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="38" max="39" width="25.6640625" customWidth="1"/>
+    <col min="40" max="40" width="28.6640625" customWidth="1"/>
+    <col min="41" max="43" width="25.6640625" customWidth="1"/>
+    <col min="44" max="44" width="31.6640625" customWidth="1"/>
+    <col min="45" max="46" width="25.6640625" customWidth="1"/>
+    <col min="47" max="48" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="49" max="53" width="25.6640625" customWidth="1"/>
+    <col min="54" max="55" width="0" hidden="1" customWidth="1"/>
+    <col min="56" max="57" width="25.6640625" customWidth="1"/>
+    <col min="58" max="59" width="0" hidden="1" customWidth="1"/>
+    <col min="60" max="61" width="25.6640625" customWidth="1"/>
+    <col min="62" max="63" width="0" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="27.6640625" customWidth="1"/>
+    <col min="65" max="65" width="26.6640625" customWidth="1"/>
+    <col min="66" max="67" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="25.6640625" customWidth="1"/>
+    <col min="69" max="69" width="23.33203125" customWidth="1"/>
+    <col min="70" max="70" width="20.6640625" customWidth="1"/>
+    <col min="71" max="71" width="20.33203125" customWidth="1"/>
+    <col min="72" max="72" width="32" customWidth="1"/>
+    <col min="73" max="73" width="16.1640625" customWidth="1"/>
+    <col min="74" max="74" width="21.5" customWidth="1"/>
+    <col min="75" max="75" width="18.83203125" customWidth="1"/>
+    <col min="76" max="76" width="19" customWidth="1"/>
+    <col min="77" max="77" width="18.83203125" customWidth="1"/>
+    <col min="78" max="78" width="16.1640625" customWidth="1"/>
+    <col min="79" max="79" width="18.33203125" customWidth="1"/>
+    <col min="80" max="80" width="18.6640625" customWidth="1"/>
+    <col min="81" max="81" width="19.5" customWidth="1"/>
+    <col min="82" max="82" width="19.33203125" customWidth="1"/>
+    <col min="83" max="83" width="24.83203125" customWidth="1"/>
+    <col min="84" max="84" width="23.5" customWidth="1"/>
+    <col min="85" max="85" width="17" customWidth="1"/>
+    <col min="86" max="86" width="16.6640625" customWidth="1"/>
+    <col min="87" max="87" width="12.5" customWidth="1"/>
+    <col min="88" max="88" width="15.33203125" customWidth="1"/>
+    <col min="89" max="89" width="13.5" customWidth="1"/>
+    <col min="90" max="90" width="15.33203125" customWidth="1"/>
+    <col min="91" max="91" width="13.83203125" customWidth="1"/>
+    <col min="92" max="92" width="15" customWidth="1"/>
+    <col min="93" max="93" width="11.83203125" customWidth="1"/>
+    <col min="94" max="99" width="16.6640625" customWidth="1"/>
+    <col min="100" max="100" width="19.5" customWidth="1"/>
+    <col min="101" max="109" width="25.6640625" customWidth="1"/>
     <col min="110" max="111" width="8.83203125" customWidth="1"/>
     <col min="112" max="112" width="25.6640625" customWidth="1"/>
-    <col min="113" max="113" width="37.6640625" customWidth="1"/>
+    <col min="113" max="114" width="8.83203125" customWidth="1"/>
+    <col min="115" max="115" width="25.6640625" customWidth="1"/>
+    <col min="116" max="116" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:119" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
@@ -13803,295 +13831,304 @@
         <v>181</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>1748</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>1749</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
         <v>1750</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>1769</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>1770</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>1771</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>1757</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>1758</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>1759</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>1694</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>1695</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>1696</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>1697</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>1698</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>1699</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>1700</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>1701</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>1702</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>1703</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>1704</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>1705</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>1706</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>1707</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>1708</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>1709</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>1710</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>1711</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>1612</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CM1" s="3" t="s">
         <v>1712</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>1613</v>
       </c>
-      <c r="CL1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>1713</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>1614</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>1714</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>1615</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>1715</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>1726</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>1725</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CV1" s="3" t="s">
         <v>1724</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CW1" s="3" t="s">
         <v>1727</v>
       </c>
-      <c r="CU1" s="3" t="s">
+      <c r="CX1" s="3" t="s">
         <v>1735</v>
       </c>
-      <c r="CV1" s="3" t="s">
+      <c r="CY1" s="3" t="s">
         <v>1736</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:116" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:119" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -14153,22 +14190,22 @@
         <v>182</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>1782</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>74</v>
@@ -14177,7 +14214,7 @@
         <v>78</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>74</v>
@@ -14195,238 +14232,238 @@
         <v>78</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>1772</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>1760</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>1761</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>1762</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="BC2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BE2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BC2" s="2" t="s">
+      <c r="BF2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BG2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BH2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="BF2" s="2" t="s">
+      <c r="BI2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BG2" s="2" t="s">
+      <c r="BJ2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BK2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="BI2" s="2" t="s">
+      <c r="BL2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="BJ2" s="2" t="s">
+      <c r="BM2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BK2" s="2" t="s">
+      <c r="BN2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BL2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BP2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BQ2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BR2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BP2" s="2" t="s">
+      <c r="BS2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="BQ2" s="2" t="s">
+      <c r="BT2" s="2" t="s">
         <v>1616</v>
       </c>
-      <c r="BR2" s="2" t="s">
+      <c r="BU2" s="2" t="s">
         <v>1617</v>
       </c>
-      <c r="BS2" s="2" t="s">
+      <c r="BV2" s="2" t="s">
         <v>1618</v>
       </c>
-      <c r="BT2" s="2" t="s">
+      <c r="BW2" s="2" t="s">
         <v>1619</v>
       </c>
-      <c r="BU2" s="2" t="s">
+      <c r="BX2" s="2" t="s">
         <v>1620</v>
       </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BY2" s="2" t="s">
         <v>1621</v>
       </c>
-      <c r="BW2" s="2" t="s">
+      <c r="BZ2" s="2" t="s">
         <v>1622</v>
       </c>
-      <c r="BX2" s="2" t="s">
+      <c r="CA2" s="2" t="s">
         <v>1623</v>
       </c>
-      <c r="BY2" s="2" t="s">
+      <c r="CB2" s="2" t="s">
         <v>1624</v>
       </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CC2" s="2" t="s">
         <v>1625</v>
       </c>
-      <c r="CA2" s="2" t="s">
+      <c r="CD2" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CE2" s="2" t="s">
         <v>1627</v>
       </c>
-      <c r="CC2" s="2" t="s">
+      <c r="CF2" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="CD2" s="2" t="s">
+      <c r="CG2" s="2" t="s">
         <v>1629</v>
       </c>
-      <c r="CE2" s="2" t="s">
+      <c r="CH2" s="2" t="s">
         <v>1630</v>
       </c>
-      <c r="CF2" s="2" t="s">
+      <c r="CI2" s="2" t="s">
         <v>1631</v>
       </c>
-      <c r="CG2" s="2" t="s">
+      <c r="CJ2" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="CH2" s="2" t="s">
+      <c r="CK2" s="2" t="s">
         <v>1633</v>
       </c>
-      <c r="CI2" s="2" t="s">
+      <c r="CL2" s="2" t="s">
         <v>1634</v>
       </c>
-      <c r="CJ2" s="2" t="s">
+      <c r="CM2" s="2" t="s">
         <v>1635</v>
       </c>
-      <c r="CK2" s="2" t="s">
+      <c r="CN2" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="CL2" s="2" t="s">
+      <c r="CO2" s="2" t="s">
         <v>1637</v>
       </c>
-      <c r="CM2" s="2" t="s">
+      <c r="CP2" s="2" t="s">
         <v>1638</v>
       </c>
-      <c r="CN2" s="2" t="s">
+      <c r="CQ2" s="2" t="s">
         <v>1639</v>
       </c>
-      <c r="CO2" s="2" t="s">
+      <c r="CR2" s="2" t="s">
         <v>1640</v>
       </c>
-      <c r="CP2" s="2" t="s">
+      <c r="CS2" s="2" t="s">
         <v>1641</v>
       </c>
-      <c r="CQ2" s="2" t="s">
+      <c r="CT2" s="2" t="s">
         <v>1722</v>
       </c>
-      <c r="CR2" s="2" t="s">
+      <c r="CU2" s="2" t="s">
         <v>1717</v>
       </c>
-      <c r="CS2" s="2" t="s">
+      <c r="CV2" s="2" t="s">
         <v>1721</v>
       </c>
-      <c r="CT2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
         <v>1728</v>
       </c>
-      <c r="CU2" s="2" t="s">
+      <c r="CX2" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="CV2" s="2" t="s">
+      <c r="CY2" s="2" t="s">
         <v>1734</v>
       </c>
-      <c r="CW2" s="2" t="s">
+      <c r="CZ2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="CX2" s="2" t="s">
+      <c r="DA2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="CY2" s="2" t="s">
+      <c r="DB2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="CZ2" s="2" t="s">
+      <c r="DC2" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="DA2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="DB2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DG2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="DE2" s="2" t="s">
+      <c r="DH2" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="DF2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="DG2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="DH2" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="DI2" s="2" t="s">
         <v>74</v>
@@ -14435,13 +14472,22 @@
         <v>78</v>
       </c>
       <c r="DK2" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="DL2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="DM2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="DN2" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="DL2" s="2" t="s">
+      <c r="DO2" s="2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="3" spans="1:116" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:119" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -14497,289 +14543,298 @@
         <v>183</v>
       </c>
       <c r="U3" s="2" t="s">
+        <v>1783</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>1784</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>1783</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>1473</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>1471</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>1472</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>1751</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>1752</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>1753</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AN3" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AM3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AN3" s="2" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AP3" s="2" t="s">
+      <c r="AS3" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AQ3" s="2" t="s">
+      <c r="AT3" s="2" t="s">
         <v>1774</v>
       </c>
-      <c r="AR3" s="2" t="s">
+      <c r="AU3" s="2" t="s">
         <v>1775</v>
       </c>
-      <c r="AS3" s="2" t="s">
+      <c r="AV3" s="2" t="s">
         <v>1774</v>
       </c>
-      <c r="AT3" s="2" t="s">
+      <c r="AW3" s="2" t="s">
         <v>1763</v>
       </c>
-      <c r="AU3" s="2" t="s">
+      <c r="AX3" s="2" t="s">
         <v>1764</v>
       </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AY3" s="2" t="s">
         <v>1765</v>
       </c>
-      <c r="AW3" s="2" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="AX3" s="2" t="s">
+      <c r="BA3" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="AY3" s="2" t="s">
+      <c r="BB3" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="AZ3" s="2" t="s">
+      <c r="BC3" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="BA3" s="2" t="s">
+      <c r="BD3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BB3" s="2" t="s">
+      <c r="BE3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="BC3" s="2" t="s">
+      <c r="BF3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BD3" s="2" t="s">
+      <c r="BG3" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="BE3" s="2" t="s">
+      <c r="BH3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="BF3" s="2" t="s">
+      <c r="BI3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="BG3" s="2" t="s">
+      <c r="BJ3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="BH3" s="2" t="s">
+      <c r="BK3" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="BI3" s="2" t="s">
+      <c r="BL3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="BJ3" s="2" t="s">
+      <c r="BM3" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="BK3" s="2" t="s">
+      <c r="BN3" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="BL3" s="2" t="s">
+      <c r="BO3" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="BM3" s="2" t="s">
+      <c r="BP3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BN3" s="2" t="s">
+      <c r="BQ3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="BO3" s="2" t="s">
+      <c r="BR3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BP3" s="2" t="s">
+      <c r="BS3" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="BQ3" s="2" t="s">
+      <c r="BT3" s="2" t="s">
         <v>1642</v>
       </c>
-      <c r="BR3" s="2" t="s">
+      <c r="BU3" s="2" t="s">
         <v>1643</v>
       </c>
-      <c r="BS3" s="2" t="s">
+      <c r="BV3" s="2" t="s">
         <v>1644</v>
       </c>
-      <c r="BT3" s="2" t="s">
+      <c r="BW3" s="2" t="s">
         <v>1645</v>
       </c>
-      <c r="BU3" s="2" t="s">
+      <c r="BX3" s="2" t="s">
         <v>1646</v>
       </c>
-      <c r="BV3" s="2" t="s">
+      <c r="BY3" s="2" t="s">
         <v>1647</v>
       </c>
-      <c r="BW3" s="2" t="s">
+      <c r="BZ3" s="2" t="s">
         <v>1648</v>
       </c>
-      <c r="BX3" s="2" t="s">
+      <c r="CA3" s="2" t="s">
         <v>1649</v>
       </c>
-      <c r="BY3" s="2" t="s">
+      <c r="CB3" s="2" t="s">
         <v>1650</v>
       </c>
-      <c r="BZ3" s="2" t="s">
+      <c r="CC3" s="2" t="s">
         <v>1651</v>
       </c>
-      <c r="CA3" s="2" t="s">
+      <c r="CD3" s="2" t="s">
         <v>1652</v>
       </c>
-      <c r="CB3" s="2" t="s">
+      <c r="CE3" s="2" t="s">
         <v>1653</v>
       </c>
-      <c r="CC3" s="2" t="s">
+      <c r="CF3" s="2" t="s">
         <v>1654</v>
       </c>
-      <c r="CD3" s="2" t="s">
+      <c r="CG3" s="2" t="s">
         <v>1655</v>
       </c>
-      <c r="CE3" s="2" t="s">
+      <c r="CH3" s="2" t="s">
         <v>1656</v>
       </c>
-      <c r="CF3" s="2" t="s">
+      <c r="CI3" s="2" t="s">
         <v>1657</v>
       </c>
-      <c r="CG3" s="2" t="s">
+      <c r="CJ3" s="2" t="s">
         <v>1658</v>
       </c>
-      <c r="CH3" s="2" t="s">
+      <c r="CK3" s="2" t="s">
         <v>1659</v>
       </c>
-      <c r="CI3" s="2" t="s">
+      <c r="CL3" s="2" t="s">
         <v>1660</v>
       </c>
-      <c r="CJ3" s="2" t="s">
+      <c r="CM3" s="2" t="s">
         <v>1661</v>
       </c>
-      <c r="CK3" s="2" t="s">
+      <c r="CN3" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="CL3" s="2" t="s">
+      <c r="CO3" s="2" t="s">
         <v>1663</v>
       </c>
-      <c r="CM3" s="2" t="s">
+      <c r="CP3" s="2" t="s">
         <v>1664</v>
       </c>
-      <c r="CN3" s="2" t="s">
+      <c r="CQ3" s="2" t="s">
         <v>1665</v>
       </c>
-      <c r="CO3" s="2" t="s">
+      <c r="CR3" s="2" t="s">
         <v>1666</v>
       </c>
-      <c r="CP3" s="2" t="s">
+      <c r="CS3" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="CQ3" s="2" t="s">
+      <c r="CT3" s="2" t="s">
         <v>1723</v>
       </c>
-      <c r="CR3" s="2" t="s">
+      <c r="CU3" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="CS3" s="2" t="s">
+      <c r="CV3" s="2" t="s">
         <v>1720</v>
       </c>
-      <c r="CT3" s="2" t="s">
+      <c r="CW3" s="2" t="s">
         <v>1729</v>
       </c>
-      <c r="CU3" s="2" t="s">
+      <c r="CX3" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="CV3" s="2" t="s">
+      <c r="CY3" s="2" t="s">
         <v>1738</v>
       </c>
-      <c r="CW3" s="2"/>
-      <c r="CX3" s="2"/>
-      <c r="CY3" s="2"/>
-      <c r="CZ3" s="2" t="s">
+      <c r="CZ3" s="2"/>
+      <c r="DA3" s="2"/>
+      <c r="DB3" s="2"/>
+      <c r="DC3" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="DA3" s="2" t="s">
+      <c r="DD3" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="DB3" s="2" t="s">
+      <c r="DE3" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="DC3" s="2" t="s">
+      <c r="DF3" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="DD3" s="2" t="s">
+      <c r="DG3" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="DE3" s="2" t="s">
+      <c r="DH3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="DF3" s="2" t="s">
+      <c r="DI3" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="DG3" s="2" t="s">
+      <c r="DJ3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="DH3" s="2" t="s">
+      <c r="DK3" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="DI3" s="2" t="s">
+      <c r="DL3" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="DJ3" s="2" t="s">
+      <c r="DM3" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="DK3" s="2" t="s">
+      <c r="DN3" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="DL3" s="2" t="s">
+      <c r="DO3" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="4" spans="1:116" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:119" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -14841,295 +14896,304 @@
         <v>184</v>
       </c>
       <c r="U4" t="s">
+        <v>1785</v>
+      </c>
+      <c r="V4" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1787</v>
+      </c>
+      <c r="X4" t="s">
         <v>188</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Y4" t="s">
         <v>192</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" t="s">
         <v>196</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AA4" t="s">
         <v>199</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>201</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AC4" t="s">
         <v>205</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AD4" t="s">
         <v>208</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AE4" t="s">
         <v>210</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AF4" t="s">
         <v>213</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AG4" t="s">
         <v>215</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AH4" t="s">
         <v>217</v>
       </c>
-      <c r="AF4" s="15" t="s">
+      <c r="AI4" s="15" t="s">
         <v>1754</v>
       </c>
-      <c r="AG4" s="15" t="s">
+      <c r="AJ4" s="15" t="s">
         <v>1755</v>
       </c>
-      <c r="AH4" s="15" t="s">
+      <c r="AK4" s="15" t="s">
         <v>1756</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AL4" t="s">
         <v>221</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AM4" t="s">
         <v>225</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AN4" t="s">
         <v>229</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AO4" t="s">
         <v>233</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AP4" t="s">
         <v>237</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AQ4" t="s">
         <v>241</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AR4" t="s">
         <v>245</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AS4" t="s">
         <v>249</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AT4" t="s">
         <v>1776</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AU4" t="s">
         <v>1777</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AV4" t="s">
         <v>1778</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AW4" t="s">
         <v>1766</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AX4" t="s">
         <v>1767</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AY4" t="s">
         <v>1768</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AZ4" t="s">
         <v>253</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BA4" t="s">
         <v>257</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BB4" t="s">
         <v>261</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BC4" t="s">
         <v>265</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BD4" t="s">
         <v>267</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BE4" t="s">
         <v>269</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BF4" t="s">
         <v>271</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BG4" t="s">
         <v>275</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BH4" t="s">
         <v>279</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BI4" t="s">
         <v>282</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BJ4" t="s">
         <v>284</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BK4" t="s">
         <v>288</v>
       </c>
-      <c r="BI4" t="s">
+      <c r="BL4" t="s">
         <v>291</v>
       </c>
-      <c r="BJ4" t="s">
+      <c r="BM4" t="s">
         <v>294</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="BN4" t="s">
         <v>296</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="BO4" t="s">
         <v>1548</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="BP4" t="s">
         <v>1549</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="BQ4" t="s">
         <v>1550</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BR4" t="s">
         <v>1551</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BS4" t="s">
         <v>1573</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="BT4" t="s">
         <v>1668</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="BU4" t="s">
         <v>1669</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="BV4" t="s">
         <v>1670</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="BW4" t="s">
         <v>1671</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="BX4" t="s">
         <v>1672</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="BY4" t="s">
         <v>1673</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="BZ4" t="s">
         <v>1674</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="CA4" t="s">
         <v>1675</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CB4" t="s">
         <v>1676</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CC4" t="s">
         <v>1677</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CD4" t="s">
         <v>1678</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CE4" t="s">
         <v>1679</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CF4" t="s">
         <v>1680</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CG4" t="s">
         <v>1681</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CH4" t="s">
         <v>1682</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CI4" t="s">
         <v>1683</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="CJ4" t="s">
         <v>1684</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CK4" t="s">
         <v>1685</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CL4" t="s">
         <v>1686</v>
       </c>
-      <c r="CJ4" t="s">
+      <c r="CM4" t="s">
         <v>1687</v>
       </c>
-      <c r="CK4" t="s">
+      <c r="CN4" t="s">
         <v>1688</v>
       </c>
-      <c r="CL4" t="s">
+      <c r="CO4" t="s">
         <v>1689</v>
       </c>
-      <c r="CM4" t="s">
+      <c r="CP4" t="s">
         <v>1690</v>
       </c>
-      <c r="CN4" t="s">
+      <c r="CQ4" t="s">
         <v>1691</v>
       </c>
-      <c r="CO4" t="s">
+      <c r="CR4" t="s">
         <v>1692</v>
       </c>
-      <c r="CP4" t="s">
+      <c r="CS4" t="s">
         <v>1693</v>
       </c>
-      <c r="CQ4" t="s">
+      <c r="CT4" t="s">
         <v>1716</v>
       </c>
-      <c r="CR4" t="s">
+      <c r="CU4" t="s">
         <v>1739</v>
       </c>
-      <c r="CS4" t="s">
+      <c r="CV4" t="s">
         <v>1719</v>
       </c>
-      <c r="CT4" t="s">
+      <c r="CW4" t="s">
         <v>1731</v>
       </c>
-      <c r="CU4" t="s">
+      <c r="CX4" t="s">
         <v>1730</v>
       </c>
-      <c r="CV4" t="s">
+      <c r="CY4" t="s">
         <v>1737</v>
       </c>
-      <c r="CW4" t="s">
+      <c r="CZ4" t="s">
         <v>308</v>
       </c>
-      <c r="CX4" t="s">
+      <c r="DA4" t="s">
         <v>311</v>
       </c>
-      <c r="CY4" t="s">
+      <c r="DB4" t="s">
         <v>314</v>
       </c>
-      <c r="CZ4" t="s">
+      <c r="DC4" t="s">
         <v>318</v>
       </c>
-      <c r="DA4" t="s">
+      <c r="DD4" t="s">
         <v>322</v>
       </c>
-      <c r="DB4" t="s">
+      <c r="DE4" t="s">
         <v>326</v>
       </c>
-      <c r="DC4" t="s">
+      <c r="DF4" t="s">
         <v>329</v>
       </c>
-      <c r="DD4" t="s">
+      <c r="DG4" t="s">
         <v>333</v>
       </c>
-      <c r="DE4" t="s">
+      <c r="DH4" t="s">
         <v>335</v>
       </c>
-      <c r="DF4" t="s">
+      <c r="DI4" t="s">
         <v>337</v>
       </c>
-      <c r="DG4" t="s">
+      <c r="DJ4" t="s">
         <v>339</v>
       </c>
-      <c r="DH4" t="s">
+      <c r="DK4" t="s">
         <v>343</v>
       </c>
-      <c r="DI4" t="s">
+      <c r="DL4" t="s">
         <v>346</v>
       </c>
-      <c r="DJ4" t="s">
+      <c r="DM4" t="s">
         <v>348</v>
       </c>
-      <c r="DK4" t="s">
+      <c r="DN4" t="s">
         <v>352</v>
       </c>
-      <c r="DL4" t="s">
+      <c r="DO4" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="5" spans="1:116" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:119" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -15163,12 +15227,12 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
@@ -15248,6 +15312,9 @@
       <c r="DJ5" s="1"/>
       <c r="DK5" s="1"/>
       <c r="DL5" s="1"/>
+      <c r="DM5" s="1"/>
+      <c r="DN5" s="1"/>
+      <c r="DO5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added digestion fields in dissociation protocol
</commit_message>
<xml_diff>
--- a/template/hca_lung_template.xlsx
+++ b/template/hca_lung_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsenios/Documents/GitHub/geo_to_hca/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA0BA11-1EFD-A545-8315-FBAE8436EB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB88B9-5351-4C49-B168-4B6189B44E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="760" windowWidth="21360" windowHeight="17600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="21360" windowHeight="17600" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3346" uniqueCount="1809">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -5426,6 +5426,69 @@
   </si>
   <si>
     <t>donor_organism.gender_identity.ontology_label</t>
+  </si>
+  <si>
+    <t>DIGESTION TIME</t>
+  </si>
+  <si>
+    <t>DIGESTION TIME UNIT</t>
+  </si>
+  <si>
+    <t>DIGESTION TIME UNIT ONTOLOGY ID</t>
+  </si>
+  <si>
+    <t>DIGESTION TIME UNIT ONTOLOGY LABEL</t>
+  </si>
+  <si>
+    <t>DIGESTION TEMPERATURE</t>
+  </si>
+  <si>
+    <t>DIGESTION SOLUTION</t>
+  </si>
+  <si>
+    <t>Time of digestion of the specimen.</t>
+  </si>
+  <si>
+    <t>The unit in which the digestion time is expressed.</t>
+  </si>
+  <si>
+    <t>Temperature of digestion in Celsius or in general terms (i.e. cold, warm, room temperature).</t>
+  </si>
+  <si>
+    <t>Enzyme(s) or reagent(s) of the solution that was used for the digestion of the specimen.</t>
+  </si>
+  <si>
+    <t>For example: 2; 5; 10</t>
+  </si>
+  <si>
+    <t>For example: second; week</t>
+  </si>
+  <si>
+    <t>For example: UO:0000010; UO:0000034</t>
+  </si>
+  <si>
+    <t>Should be either numeric value or one of frozen, cold, room temperature, warm. For example: 4; 37; cold</t>
+  </si>
+  <si>
+    <t>Should be of: Citric-acid based, Detergent-based, Lysis buffer, Accutase, Collagenase, Collagenase A, Collagenase D, Collagenase I, Collagenase II, Collagenase IV, Dispase, Dispase II, DNAse I, Elastase, Hyaluronidase, Liberase, Papain, Protease, TrypLE, Trypsin</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.digestion_time</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.digestion_time_unit.text</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.digestion_time_unit.ontology</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.digestion_time_unit.ontology_label</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.digestion_temperature</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.digestion_solution</t>
   </si>
 </sst>
 </file>
@@ -9680,9 +9743,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9692,10 +9757,15 @@
     <col min="4" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
     <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="15" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" customWidth="1"/>
+    <col min="12" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="21" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>577</v>
       </c>
@@ -9724,25 +9794,43 @@
         <v>892</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>1792</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>1793</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>875</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>473</v>
       </c>
@@ -9771,25 +9859,43 @@
         <v>78</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>1794</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>1795</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>1796</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>1797</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>474</v>
       </c>
@@ -9814,25 +9920,43 @@
         <v>342</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>1798</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1799</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1800</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>1799</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>1801</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>1802</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>578</v>
       </c>
@@ -9861,25 +9985,43 @@
         <v>893</v>
       </c>
       <c r="J4" t="s">
+        <v>1803</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1804</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1805</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1806</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1807</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1808</v>
+      </c>
+      <c r="P4" t="s">
         <v>894</v>
       </c>
-      <c r="K4" t="s">
+      <c r="Q4" t="s">
         <v>895</v>
       </c>
-      <c r="L4" t="s">
+      <c r="R4" t="s">
         <v>896</v>
       </c>
-      <c r="M4" t="s">
+      <c r="S4" t="s">
         <v>897</v>
       </c>
-      <c r="N4" t="s">
+      <c r="T4" t="s">
         <v>898</v>
       </c>
-      <c r="O4" t="s">
+      <c r="U4" t="s">
         <v>899</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -9897,6 +10039,12 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13692,7 +13840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:DO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V5" sqref="V5:W5"/>
     </sheetView>
   </sheetViews>

</xml_diff>